<commit_message>
chirp signals and trials
</commit_message>
<xml_diff>
--- a/doc/ForceTendon.xlsx
+++ b/doc/ForceTendon.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21765" windowHeight="12435" activeTab="1"/>
+    <workbookView windowWidth="21765" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Values" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
   <si>
     <t>Posterior</t>
   </si>
@@ -46,16 +46,19 @@
   <si>
     <t>Pretension</t>
   </si>
+  <si>
+    <t>DIa 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -66,27 +69,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -104,16 +91,75 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -128,7 +174,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -136,77 +181,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -219,7 +222,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,49 +318,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,121 +402,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -428,50 +431,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,6 +481,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -525,153 +504,177 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1305,7 +1308,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$D$14:$D$21</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>3.87097</c:v>
@@ -1328,7 +1331,7 @@
                 <c:pt idx="6">
                   <c:v>4.05181</c:v>
                 </c:pt>
-                <c:pt idx="7" c:formatCode="General">
+                <c:pt idx="7">
                   <c:v>4.08602</c:v>
                 </c:pt>
               </c:numCache>
@@ -1419,7 +1422,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0.00000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3071,8 +3074,8 @@
   <sheetPr/>
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="5"/>
@@ -3173,15 +3176,15 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2">
         <f>A5*COS(PI()/2-RADIANS($B$2))</f>
-        <v>74.6864341197761</v>
+        <v>9.33580426497202</v>
       </c>
       <c r="C5" s="1">
         <f>0.0246*B5/9.8+$D$2</f>
-        <v>1.98607819177005</v>
+        <v>1.82203477397126</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="2">
@@ -3199,15 +3202,15 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2">
-        <v>120</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <f>A6*COS(PI()/2-RADIANS($B$2))</f>
-        <v>112.029651179664</v>
+        <v>4.66790213248601</v>
       </c>
       <c r="C6" s="1">
         <f>0.0246*B6/9.8+$D$2</f>
-        <v>2.07981728765508</v>
+        <v>1.81031738698563</v>
       </c>
       <c r="D6" s="1"/>
       <c r="F6" s="2">
@@ -3245,13 +3248,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="12.5"/>
     <col min="3" max="3" width="11.8" customWidth="1"/>
@@ -3337,6 +3340,37 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1.83</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1.8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>3.93</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>3.91</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Loadcell characterization and package updated
</commit_message>
<xml_diff>
--- a/doc/ForceTendon.xlsx
+++ b/doc/ForceTendon.xlsx
@@ -61,10 +61,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -90,13 +90,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -105,40 +98,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,9 +115,48 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -168,8 +168,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,15 +184,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,10 +212,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -234,6 +234,126 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -246,7 +366,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,103 +384,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,49 +402,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,26 +437,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,17 +496,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -525,153 +534,144 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3256,8 +3256,8 @@
   <sheetPr/>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
@@ -3389,27 +3389,25 @@
         <v>2</v>
       </c>
       <c r="B16" s="2">
-        <f>180-116</f>
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="2">
-        <v>1.8181</v>
+        <v>1.81</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G16" s="2">
-        <f>180-98</f>
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I16" s="2">
-        <v>3.157</v>
+        <v>3.43</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -3440,24 +3438,23 @@
       </c>
       <c r="B18" s="2">
         <f>A18*COS(PI()/2-RADIANS($B$16))</f>
-        <v>17.9758809259833</v>
+        <v>19.8053613748314</v>
       </c>
       <c r="C18" s="1">
         <f>0.0006506158*B18+$D$16</f>
-        <v>1.82979539214936</v>
+        <v>1.82288568103518</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="E18"/>
       <c r="F18" s="2">
         <v>20</v>
       </c>
       <c r="G18" s="2">
         <f>F18*COS(PI()/2-RADIANS($G$16))</f>
-        <v>19.8053613748314</v>
+        <v>19.8509230328264</v>
       </c>
       <c r="H18" s="1">
         <f>0.0003329729*G18+$I$16</f>
-        <v>3.16359464861253</v>
+        <v>3.43660981940992</v>
       </c>
       <c r="I18" s="1"/>
     </row>
@@ -3467,11 +3464,11 @@
       </c>
       <c r="B19" s="2">
         <f>A19*COS(PI()/2-RADIANS($B$16))</f>
-        <v>71.9035237039334</v>
+        <v>79.2214454993256</v>
       </c>
       <c r="C19" s="1">
         <f>0.0006506158*B19+$D$16</f>
-        <v>1.86488156859745</v>
+        <v>1.8615427241407</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="2">
@@ -3479,11 +3476,11 @@
       </c>
       <c r="G19" s="2">
         <f>F19*COS(PI()/2-RADIANS($G$16))</f>
-        <v>79.2214454993256</v>
+        <v>79.4036921313058</v>
       </c>
       <c r="H19" s="1">
         <f>0.0003329729*G19+$I$16</f>
-        <v>3.1833785944501</v>
+        <v>3.45643927763967</v>
       </c>
       <c r="I19" s="1"/>
     </row>
@@ -3493,11 +3490,11 @@
       </c>
       <c r="B20" s="2">
         <f>A20*COS(PI()/2-RADIANS($B$16))</f>
-        <v>107.8552855559</v>
+        <v>118.832168248988</v>
       </c>
       <c r="C20" s="1">
         <f>0.0006506158*B20+$D$16</f>
-        <v>1.88827235289618</v>
+        <v>1.88731408621105</v>
       </c>
       <c r="D20" s="1"/>
       <c r="F20" s="2">
@@ -3505,11 +3502,11 @@
       </c>
       <c r="G20" s="2">
         <f>F20*COS(PI()/2-RADIANS($G$16))</f>
-        <v>118.832168248988</v>
+        <v>119.105538196959</v>
       </c>
       <c r="H20" s="1">
         <f>0.0003329729*G20+$I$16</f>
-        <v>3.19656789167515</v>
+        <v>3.4696589164595</v>
       </c>
       <c r="I20" s="1"/>
     </row>

</xml_diff>